<commit_message>
upgrade to new version
</commit_message>
<xml_diff>
--- a/tests/data/codes/test-002.xlsx
+++ b/tests/data/codes/test-002.xlsx
@@ -7,8 +7,8 @@
     <workbookView windowWidth="20308" windowHeight="7734" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="relation" sheetId="1" r:id="rId1"/>
-    <sheet name="attr" sheetId="2" r:id="rId2"/>
+    <sheet name="Relations" sheetId="1" r:id="rId1"/>
+    <sheet name="Attrs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -46,10 +46,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -60,6 +60,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -68,17 +75,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -115,23 +131,46 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -143,9 +182,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,54 +198,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -213,13 +213,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,49 +363,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,115 +375,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,26 +446,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,11 +474,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -504,153 +489,168 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -658,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -840,7 +840,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -864,9 +864,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -890,7 +890,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -943,7 +943,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -968,7 +968,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1035,7 +1035,7 @@
   <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7972972972973" defaultRowHeight="17.05" outlineLevelRow="7"/>

</xml_diff>